<commit_message>
update import export excel api
</commit_message>
<xml_diff>
--- a/static/business.xlsx
+++ b/static/business.xlsx
@@ -1,55 +1,112 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
   <workbookPr codeName="ThisWorkbook"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/phitrunghieu/Downloads/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAF82063-5EA1-DA44-89EC-9370D387D652}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
   </sheets>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
-<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
-  <metadataTypes count="1">
-    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
-  </metadataTypes>
-  <futureMetadata name="XLDAPR" count="1">
-    <bk>
-      <extLst>
-        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
-          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
-        </ext>
-      </extLst>
-    </bk>
-  </futureMetadata>
-  <cellMetadata count="1">
-    <bk>
-      <rc t="1" v="0"/>
-    </bk>
-  </cellMetadata>
-</metadata>
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+  <si>
+    <t>EMAIL</t>
+  </si>
+  <si>
+    <t>GHI CHÚ</t>
+  </si>
+  <si>
+    <t>TÊN DOANH NGHIỆP</t>
+  </si>
+  <si>
+    <t>LĨNH VỰC KINH DOANH</t>
+  </si>
+  <si>
+    <t>ĐIỆN THOẠI</t>
+  </si>
+  <si>
+    <t>QUỐC GIA</t>
+  </si>
+  <si>
+    <t>CHI TIẾT LIÊN HỆ</t>
+  </si>
+  <si>
+    <t>ĐỊA CHỈ XUẤT/NHẬP KHẢU</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:vt="http://schemas.openxmlformats.org/officeDocument/2006/docPropsVTypes">
-  <numFmts count="1">
-    <numFmt numFmtId="56" formatCode="&quot;上午/下午 &quot;hh&quot;時&quot;mm&quot;分&quot;ss&quot;秒 &quot;"/>
-  </numFmts>
-  <fonts count="1">
-    <font>
-      <sz val="12"/>
-      <color theme="1"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="6" x14ac:knownFonts="1">
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF008B8B"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -61,17 +118,35 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+  <cellStyleXfs count="2">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyBorder="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+  <cellXfs count="7">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -150,7 +225,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -185,7 +259,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -220,16 +293,20 @@
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:tint val="100000"/>
-                <a:shade val="100000"/>
+                <a:shade val="51000"/>
                 <a:satMod val="130000"/>
               </a:schemeClr>
             </a:gs>
+            <a:gs pos="80000">
+              <a:schemeClr val="phClr">
+                <a:shade val="93000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:tint val="50000"/>
-                <a:shade val="100000"/>
-                <a:satMod val="350000"/>
+                <a:shade val="94000"/>
+                <a:satMod val="135000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
@@ -351,92 +428,65 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
-  <a:objectDefaults>
-    <a:spDef>
-      <a:spPr/>
-      <a:bodyPr/>
-      <a:lstStyle/>
-      <a:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="3">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="2">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </a:style>
-    </a:spDef>
-    <a:lnDef>
-      <a:spPr/>
-      <a:bodyPr/>
-      <a:lstStyle/>
-      <a:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </a:style>
-    </a:lnDef>
-  </a:objectDefaults>
+  <a:objectDefaults/>
   <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
+    </sheetView>
   </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="23" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.6640625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="25.6640625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="15.6640625" style="1" customWidth="1"/>
+    <col min="6" max="7" width="20.6640625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="30.6640625" style="1" customWidth="1"/>
+    <col min="9" max="16384" width="9.1640625" style="1"/>
+  </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" t="str">
-        <v>businessName</v>
-      </c>
-      <c r="B1" t="str">
-        <v>businessType</v>
-      </c>
-      <c r="C1" t="str">
-        <v>businessAreaId</v>
-      </c>
-      <c r="D1" t="str">
-        <v>businessAddress</v>
-      </c>
-      <c r="E1" t="str">
-        <v>businessEmail</v>
-      </c>
-      <c r="F1" t="str">
-        <v>businessPhone</v>
-      </c>
-      <c r="G1" t="str">
-        <v>country</v>
-      </c>
-      <c r="H1" t="str">
-        <v>contactDeatail</v>
-      </c>
-      <c r="I1" t="str">
-        <v>note</v>
-      </c>
-      <c r="J1" t="str">
-        <v>status</v>
-      </c>
+    <row r="1" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B2" s="6"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="5"/>
+      <c r="G2" s="6"/>
     </row>
   </sheetData>
-  <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:J1"/>
-  </ignoredErrors>
+  <pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>